<commit_message>
Reading data and formulas complete
</commit_message>
<xml_diff>
--- a/DewateringData-SelectedSheets.xlsx
+++ b/DewateringData-SelectedSheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Dewatering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F6853D-D9D5-4D5D-8654-A41EEE1585CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255D3A86-5F03-496B-AB56-F5CA8EBAF519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="05_28_2020" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'05_21_2020'!$U$5:$AK$61</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'05_28_2020'!$U$5:$AL$61</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2087,19 +2087,16 @@
     <xf numFmtId="2" fontId="12" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2117,16 +2114,19 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5802,46 +5802,46 @@
   </sheetPr>
   <dimension ref="A1:BF76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="16.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="16.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="2" customWidth="1"/>
     <col min="15" max="15" width="11" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" style="2" customWidth="1"/>
     <col min="17" max="17" width="11" style="2" customWidth="1"/>
-    <col min="18" max="21" width="11.6640625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="22.33203125" style="2" customWidth="1"/>
-    <col min="23" max="25" width="11.6640625" style="2" customWidth="1"/>
-    <col min="26" max="26" width="21.33203125" style="2" customWidth="1"/>
-    <col min="27" max="35" width="11.6640625" style="2" customWidth="1"/>
-    <col min="36" max="36" width="13.33203125" style="2" customWidth="1"/>
-    <col min="37" max="37" width="14.6640625" style="2" customWidth="1"/>
-    <col min="38" max="38" width="11.6640625" style="2" customWidth="1"/>
-    <col min="39" max="39" width="9.44140625" style="2" customWidth="1"/>
-    <col min="40" max="40" width="8.33203125" style="2" customWidth="1"/>
-    <col min="41" max="41" width="7.44140625" style="2" customWidth="1"/>
-    <col min="42" max="43" width="9.33203125" style="2" customWidth="1"/>
-    <col min="44" max="44" width="8.44140625" style="2" customWidth="1"/>
-    <col min="45" max="64" width="9.33203125" style="2" customWidth="1"/>
-    <col min="65" max="16384" width="8.6640625" style="2"/>
+    <col min="18" max="21" width="11.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="22.28515625" style="2" customWidth="1"/>
+    <col min="23" max="25" width="11.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="21.28515625" style="2" customWidth="1"/>
+    <col min="27" max="35" width="11.7109375" style="2" customWidth="1"/>
+    <col min="36" max="36" width="13.28515625" style="2" customWidth="1"/>
+    <col min="37" max="37" width="14.7109375" style="2" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" style="2" customWidth="1"/>
+    <col min="39" max="39" width="9.42578125" style="2" customWidth="1"/>
+    <col min="40" max="40" width="8.28515625" style="2" customWidth="1"/>
+    <col min="41" max="41" width="7.42578125" style="2" customWidth="1"/>
+    <col min="42" max="43" width="9.28515625" style="2" customWidth="1"/>
+    <col min="44" max="44" width="8.42578125" style="2" customWidth="1"/>
+    <col min="45" max="64" width="9.28515625" style="2" customWidth="1"/>
+    <col min="65" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -5903,7 +5903,7 @@
       <c r="BE1" s="4"/>
       <c r="BF1" s="4"/>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -5965,7 +5965,7 @@
       <c r="BE2" s="4"/>
       <c r="BF2" s="4"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>2</v>
@@ -6027,7 +6027,7 @@
       <c r="BE3" s="4"/>
       <c r="BF3" s="4"/>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -6087,7 +6087,7 @@
       <c r="BE4" s="4"/>
       <c r="BF4" s="4"/>
     </row>
-    <row r="5" spans="1:58" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -6108,26 +6108,26 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
-      <c r="U5" s="185" t="s">
+      <c r="U5" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="V5" s="185"/>
-      <c r="W5" s="185"/>
-      <c r="X5" s="185"/>
-      <c r="Y5" s="185"/>
-      <c r="Z5" s="185"/>
-      <c r="AA5" s="185"/>
-      <c r="AB5" s="185"/>
-      <c r="AC5" s="185"/>
-      <c r="AD5" s="185"/>
-      <c r="AE5" s="185"/>
-      <c r="AF5" s="185"/>
-      <c r="AG5" s="185"/>
-      <c r="AH5" s="185"/>
-      <c r="AI5" s="185"/>
-      <c r="AJ5" s="185"/>
-      <c r="AK5" s="185"/>
-      <c r="AL5" s="185"/>
+      <c r="V5" s="175"/>
+      <c r="W5" s="175"/>
+      <c r="X5" s="175"/>
+      <c r="Y5" s="175"/>
+      <c r="Z5" s="175"/>
+      <c r="AA5" s="175"/>
+      <c r="AB5" s="175"/>
+      <c r="AC5" s="175"/>
+      <c r="AD5" s="175"/>
+      <c r="AE5" s="175"/>
+      <c r="AF5" s="175"/>
+      <c r="AG5" s="175"/>
+      <c r="AH5" s="175"/>
+      <c r="AI5" s="175"/>
+      <c r="AJ5" s="175"/>
+      <c r="AK5" s="175"/>
+      <c r="AL5" s="175"/>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
       <c r="AO5" s="4"/>
@@ -6149,7 +6149,7 @@
       <c r="BE5" s="4"/>
       <c r="BF5" s="4"/>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -6170,24 +6170,24 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
-      <c r="U6" s="185"/>
-      <c r="V6" s="185"/>
-      <c r="W6" s="185"/>
-      <c r="X6" s="185"/>
-      <c r="Y6" s="185"/>
-      <c r="Z6" s="185"/>
-      <c r="AA6" s="185"/>
-      <c r="AB6" s="185"/>
-      <c r="AC6" s="185"/>
-      <c r="AD6" s="185"/>
-      <c r="AE6" s="185"/>
-      <c r="AF6" s="185"/>
-      <c r="AG6" s="185"/>
-      <c r="AH6" s="185"/>
-      <c r="AI6" s="185"/>
-      <c r="AJ6" s="185"/>
-      <c r="AK6" s="185"/>
-      <c r="AL6" s="185"/>
+      <c r="U6" s="175"/>
+      <c r="V6" s="175"/>
+      <c r="W6" s="175"/>
+      <c r="X6" s="175"/>
+      <c r="Y6" s="175"/>
+      <c r="Z6" s="175"/>
+      <c r="AA6" s="175"/>
+      <c r="AB6" s="175"/>
+      <c r="AC6" s="175"/>
+      <c r="AD6" s="175"/>
+      <c r="AE6" s="175"/>
+      <c r="AF6" s="175"/>
+      <c r="AG6" s="175"/>
+      <c r="AH6" s="175"/>
+      <c r="AI6" s="175"/>
+      <c r="AJ6" s="175"/>
+      <c r="AK6" s="175"/>
+      <c r="AL6" s="175"/>
       <c r="AM6" s="4"/>
       <c r="AN6" s="4"/>
       <c r="AO6" s="4"/>
@@ -6209,13 +6209,13 @@
       <c r="BE6" s="4"/>
       <c r="BF6" s="4"/>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A7" s="186" t="s">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A7" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="186"/>
-      <c r="C7" s="186"/>
-      <c r="D7" s="186"/>
+      <c r="B7" s="176"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
       <c r="E7" s="4"/>
       <c r="F7" s="8" t="s">
         <v>5</v>
@@ -6234,24 +6234,24 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
-      <c r="U7" s="185"/>
-      <c r="V7" s="185"/>
-      <c r="W7" s="185"/>
-      <c r="X7" s="185"/>
-      <c r="Y7" s="185"/>
-      <c r="Z7" s="185"/>
-      <c r="AA7" s="185"/>
-      <c r="AB7" s="185"/>
-      <c r="AC7" s="185"/>
-      <c r="AD7" s="185"/>
-      <c r="AE7" s="185"/>
-      <c r="AF7" s="185"/>
-      <c r="AG7" s="185"/>
-      <c r="AH7" s="185"/>
-      <c r="AI7" s="185"/>
-      <c r="AJ7" s="185"/>
-      <c r="AK7" s="185"/>
-      <c r="AL7" s="185"/>
+      <c r="U7" s="175"/>
+      <c r="V7" s="175"/>
+      <c r="W7" s="175"/>
+      <c r="X7" s="175"/>
+      <c r="Y7" s="175"/>
+      <c r="Z7" s="175"/>
+      <c r="AA7" s="175"/>
+      <c r="AB7" s="175"/>
+      <c r="AC7" s="175"/>
+      <c r="AD7" s="175"/>
+      <c r="AE7" s="175"/>
+      <c r="AF7" s="175"/>
+      <c r="AG7" s="175"/>
+      <c r="AH7" s="175"/>
+      <c r="AI7" s="175"/>
+      <c r="AJ7" s="175"/>
+      <c r="AK7" s="175"/>
+      <c r="AL7" s="175"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
@@ -6273,7 +6273,7 @@
       <c r="BE7" s="4"/>
       <c r="BF7" s="4"/>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
@@ -6344,7 +6344,7 @@
       <c r="BE8" s="4"/>
       <c r="BF8" s="4"/>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
@@ -6421,7 +6421,7 @@
       <c r="BE9" s="4"/>
       <c r="BF9" s="4"/>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>16</v>
       </c>
@@ -6497,7 +6497,7 @@
       <c r="BE10" s="4"/>
       <c r="BF10" s="4"/>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -6579,7 +6579,7 @@
       <c r="BE11" s="4"/>
       <c r="BF11" s="4"/>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -6661,7 +6661,7 @@
       <c r="BE12" s="4"/>
       <c r="BF12" s="4"/>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>28</v>
       </c>
@@ -6743,7 +6743,7 @@
       <c r="BE13" s="4"/>
       <c r="BF13" s="4"/>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>31</v>
       </c>
@@ -6825,7 +6825,7 @@
       <c r="BE14" s="4"/>
       <c r="BF14" s="4"/>
     </row>
-    <row r="15" spans="1:58" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:58" ht="31.5" x14ac:dyDescent="0.4">
       <c r="A15" s="39" t="s">
         <v>35</v>
       </c>
@@ -6894,7 +6894,7 @@
       <c r="BE15" s="4"/>
       <c r="BF15" s="4"/>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16" s="43"/>
       <c r="B16" s="43"/>
       <c r="C16" s="4"/>
@@ -6954,12 +6954,12 @@
       <c r="BE16" s="4"/>
       <c r="BF16" s="4"/>
     </row>
-    <row r="17" spans="1:58" ht="15.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A17" s="187" t="s">
+    <row r="17" spans="1:58" ht="15.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A17" s="177" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="187"/>
-      <c r="C17" s="187"/>
+      <c r="B17" s="177"/>
+      <c r="C17" s="177"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -7016,7 +7016,7 @@
       <c r="BE17" s="4"/>
       <c r="BF17" s="4"/>
     </row>
-    <row r="18" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="12"/>
       <c r="C18" s="45"/>
@@ -7076,12 +7076,11 @@
       <c r="BE18" s="4"/>
       <c r="BF18" s="4"/>
     </row>
-    <row r="19" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="47">
-        <f>1/453.59237</f>
         <v>2.2046226218487759E-3</v>
       </c>
       <c r="C19" s="48" t="s">
@@ -7143,7 +7142,7 @@
       <c r="BE19" s="4"/>
       <c r="BF19" s="4"/>
     </row>
-    <row r="20" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
         <v>38</v>
       </c>
@@ -7209,7 +7208,7 @@
       <c r="BE20" s="4"/>
       <c r="BF20" s="4"/>
     </row>
-    <row r="21" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
         <v>41</v>
       </c>
@@ -7275,7 +7274,7 @@
       <c r="BE21" s="4"/>
       <c r="BF21" s="4"/>
     </row>
-    <row r="22" spans="1:58" ht="17.399999999999999" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:58" ht="18" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
         <v>43</v>
       </c>
@@ -7342,12 +7341,12 @@
       <c r="BE22" s="4"/>
       <c r="BF22" s="4"/>
     </row>
-    <row r="23" spans="1:58" ht="17.399999999999999" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A23" s="188" t="s">
+    <row r="23" spans="1:58" ht="18" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A23" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="188"/>
-      <c r="C23" s="188"/>
+      <c r="B23" s="178"/>
+      <c r="C23" s="178"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -7404,7 +7403,7 @@
       <c r="BE23" s="4"/>
       <c r="BF23" s="4"/>
     </row>
-    <row r="24" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
         <v>46</v>
       </c>
@@ -7471,7 +7470,7 @@
       <c r="BE24" s="4"/>
       <c r="BF24" s="4"/>
     </row>
-    <row r="25" spans="1:58" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:58" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
         <v>48</v>
       </c>
@@ -7537,12 +7536,12 @@
       <c r="BE25" s="4"/>
       <c r="BF25" s="4"/>
     </row>
-    <row r="26" spans="1:58" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A26" s="188" t="s">
+    <row r="26" spans="1:58" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A26" s="178" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="188"/>
-      <c r="C26" s="188"/>
+      <c r="B26" s="178"/>
+      <c r="C26" s="178"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -7599,7 +7598,7 @@
       <c r="BE26" s="4"/>
       <c r="BF26" s="4"/>
     </row>
-    <row r="27" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
         <v>51</v>
       </c>
@@ -7662,7 +7661,7 @@
       <c r="BD27" s="4"/>
       <c r="BE27" s="4"/>
     </row>
-    <row r="28" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="51" t="s">
         <v>52</v>
       </c>
@@ -7727,7 +7726,7 @@
       <c r="BD28" s="4"/>
       <c r="BE28" s="4"/>
     </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -7786,7 +7785,7 @@
       <c r="BD29" s="4"/>
       <c r="BE29" s="4"/>
     </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -7845,27 +7844,27 @@
       <c r="BD30" s="4"/>
       <c r="BE30" s="4"/>
     </row>
-    <row r="31" spans="1:58" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="180" t="s">
+    <row r="31" spans="1:58" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="179" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="180"/>
-      <c r="C31" s="180"/>
-      <c r="D31" s="180"/>
-      <c r="E31" s="180"/>
-      <c r="F31" s="180"/>
-      <c r="G31" s="180"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="180"/>
-      <c r="J31" s="180"/>
-      <c r="K31" s="180"/>
-      <c r="L31" s="180"/>
-      <c r="M31" s="180"/>
-      <c r="N31" s="180"/>
-      <c r="O31" s="180"/>
-      <c r="P31" s="180"/>
-      <c r="Q31" s="180"/>
-      <c r="R31" s="180"/>
+      <c r="B31" s="179"/>
+      <c r="C31" s="179"/>
+      <c r="D31" s="179"/>
+      <c r="E31" s="179"/>
+      <c r="F31" s="179"/>
+      <c r="G31" s="179"/>
+      <c r="H31" s="179"/>
+      <c r="I31" s="179"/>
+      <c r="J31" s="179"/>
+      <c r="K31" s="179"/>
+      <c r="L31" s="179"/>
+      <c r="M31" s="179"/>
+      <c r="N31" s="179"/>
+      <c r="O31" s="179"/>
+      <c r="P31" s="179"/>
+      <c r="Q31" s="179"/>
+      <c r="R31" s="179"/>
       <c r="S31" s="54"/>
       <c r="T31" s="54"/>
       <c r="U31" s="26"/>
@@ -7906,7 +7905,7 @@
       <c r="BD31" s="4"/>
       <c r="BE31" s="4"/>
     </row>
-    <row r="32" spans="1:58" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:58" ht="63" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
         <v>56</v>
       </c>
@@ -8001,7 +8000,7 @@
       <c r="BD32" s="4"/>
       <c r="BE32" s="4"/>
     </row>
-    <row r="33" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A33" s="59">
         <v>1</v>
       </c>
@@ -8104,7 +8103,7 @@
       <c r="BD33" s="4"/>
       <c r="BE33" s="4"/>
     </row>
-    <row r="34" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A34" s="59">
         <v>2</v>
       </c>
@@ -8207,7 +8206,7 @@
       <c r="BD34" s="4"/>
       <c r="BE34" s="4"/>
     </row>
-    <row r="35" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A35" s="59">
         <v>3</v>
       </c>
@@ -8309,7 +8308,7 @@
       <c r="BD35" s="4"/>
       <c r="BE35" s="4"/>
     </row>
-    <row r="36" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A36" s="59">
         <v>4</v>
       </c>
@@ -8411,7 +8410,7 @@
       <c r="BD36" s="4"/>
       <c r="BE36" s="4"/>
     </row>
-    <row r="37" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A37" s="59">
         <v>5</v>
       </c>
@@ -8513,7 +8512,7 @@
       <c r="BD37" s="4"/>
       <c r="BE37" s="4"/>
     </row>
-    <row r="38" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A38" s="70">
         <v>6</v>
       </c>
@@ -8615,22 +8614,22 @@
       <c r="BD38" s="4"/>
       <c r="BE38" s="4"/>
     </row>
-    <row r="39" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="181" t="s">
+    <row r="39" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="180" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="181"/>
-      <c r="C39" s="181"/>
-      <c r="D39" s="181"/>
-      <c r="E39" s="181"/>
-      <c r="F39" s="181"/>
-      <c r="G39" s="181"/>
-      <c r="H39" s="181"/>
-      <c r="I39" s="181"/>
-      <c r="J39" s="181"/>
-      <c r="K39" s="181"/>
-      <c r="L39" s="181"/>
-      <c r="M39" s="181"/>
+      <c r="B39" s="180"/>
+      <c r="C39" s="180"/>
+      <c r="D39" s="180"/>
+      <c r="E39" s="180"/>
+      <c r="F39" s="180"/>
+      <c r="G39" s="180"/>
+      <c r="H39" s="180"/>
+      <c r="I39" s="180"/>
+      <c r="J39" s="180"/>
+      <c r="K39" s="180"/>
+      <c r="L39" s="180"/>
+      <c r="M39" s="180"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
@@ -8678,7 +8677,7 @@
       <c r="BD39" s="4"/>
       <c r="BE39" s="4"/>
     </row>
-    <row r="40" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="56" t="s">
         <v>56</v>
       </c>
@@ -8688,20 +8687,20 @@
       <c r="C40" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="182" t="s">
+      <c r="D40" s="181" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="182"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="182"/>
-      <c r="H40" s="182"/>
-      <c r="I40" s="183" t="s">
+      <c r="E40" s="181"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="181"/>
+      <c r="H40" s="181"/>
+      <c r="I40" s="182" t="s">
         <v>78</v>
       </c>
-      <c r="J40" s="183"/>
-      <c r="K40" s="183"/>
-      <c r="L40" s="183"/>
-      <c r="M40" s="183"/>
+      <c r="J40" s="182"/>
+      <c r="K40" s="182"/>
+      <c r="L40" s="182"/>
+      <c r="M40" s="182"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
@@ -8747,7 +8746,7 @@
       <c r="BD40" s="4"/>
       <c r="BE40" s="4"/>
     </row>
-    <row r="41" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A41" s="74">
         <v>1</v>
       </c>
@@ -8824,7 +8823,7 @@
       <c r="BD41" s="4"/>
       <c r="BE41" s="4"/>
     </row>
-    <row r="42" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A42" s="74">
         <v>2</v>
       </c>
@@ -8901,7 +8900,7 @@
       <c r="BD42" s="4"/>
       <c r="BE42" s="4"/>
     </row>
-    <row r="43" spans="1:57" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:57" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="74">
         <v>3</v>
       </c>
@@ -8942,28 +8941,28 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
-      <c r="U43" s="184" t="s">
+      <c r="U43" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="V43" s="184"/>
-      <c r="W43" s="184"/>
-      <c r="X43" s="184"/>
-      <c r="Y43" s="184"/>
-      <c r="Z43" s="184"/>
-      <c r="AA43" s="184"/>
-      <c r="AB43" s="184"/>
-      <c r="AC43" s="184"/>
-      <c r="AD43" s="175" t="s">
+      <c r="V43" s="183"/>
+      <c r="W43" s="183"/>
+      <c r="X43" s="183"/>
+      <c r="Y43" s="183"/>
+      <c r="Z43" s="183"/>
+      <c r="AA43" s="183"/>
+      <c r="AB43" s="183"/>
+      <c r="AC43" s="183"/>
+      <c r="AD43" s="184" t="s">
         <v>80</v>
       </c>
-      <c r="AE43" s="175"/>
-      <c r="AF43" s="175"/>
-      <c r="AG43" s="175"/>
-      <c r="AH43" s="175"/>
-      <c r="AI43" s="175"/>
-      <c r="AJ43" s="175"/>
-      <c r="AK43" s="175"/>
-      <c r="AL43" s="175"/>
+      <c r="AE43" s="184"/>
+      <c r="AF43" s="184"/>
+      <c r="AG43" s="184"/>
+      <c r="AH43" s="184"/>
+      <c r="AI43" s="184"/>
+      <c r="AJ43" s="184"/>
+      <c r="AK43" s="184"/>
+      <c r="AL43" s="184"/>
       <c r="AM43" s="4"/>
       <c r="AN43" s="4"/>
       <c r="AO43" s="4"/>
@@ -8984,7 +8983,7 @@
       <c r="BD43" s="4"/>
       <c r="BE43" s="4"/>
     </row>
-    <row r="44" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="74">
         <v>4</v>
       </c>
@@ -9025,24 +9024,24 @@
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
-      <c r="U44" s="184"/>
-      <c r="V44" s="184"/>
-      <c r="W44" s="184"/>
-      <c r="X44" s="184"/>
-      <c r="Y44" s="184"/>
-      <c r="Z44" s="184"/>
-      <c r="AA44" s="184"/>
-      <c r="AB44" s="184"/>
-      <c r="AC44" s="184"/>
-      <c r="AD44" s="175"/>
-      <c r="AE44" s="175"/>
-      <c r="AF44" s="175"/>
-      <c r="AG44" s="175"/>
-      <c r="AH44" s="175"/>
-      <c r="AI44" s="175"/>
-      <c r="AJ44" s="175"/>
-      <c r="AK44" s="175"/>
-      <c r="AL44" s="175"/>
+      <c r="U44" s="183"/>
+      <c r="V44" s="183"/>
+      <c r="W44" s="183"/>
+      <c r="X44" s="183"/>
+      <c r="Y44" s="183"/>
+      <c r="Z44" s="183"/>
+      <c r="AA44" s="183"/>
+      <c r="AB44" s="183"/>
+      <c r="AC44" s="183"/>
+      <c r="AD44" s="184"/>
+      <c r="AE44" s="184"/>
+      <c r="AF44" s="184"/>
+      <c r="AG44" s="184"/>
+      <c r="AH44" s="184"/>
+      <c r="AI44" s="184"/>
+      <c r="AJ44" s="184"/>
+      <c r="AK44" s="184"/>
+      <c r="AL44" s="184"/>
       <c r="AM44" s="4"/>
       <c r="AN44" s="4"/>
       <c r="AO44" s="4"/>
@@ -9063,7 +9062,7 @@
       <c r="BD44" s="4"/>
       <c r="BE44" s="4"/>
     </row>
-    <row r="45" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="74">
         <v>5</v>
       </c>
@@ -9142,7 +9141,7 @@
       <c r="BD45" s="4"/>
       <c r="BE45" s="4"/>
     </row>
-    <row r="46" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="74">
         <v>6</v>
       </c>
@@ -9221,7 +9220,7 @@
       <c r="BD46" s="4"/>
       <c r="BE46" s="4"/>
     </row>
-    <row r="47" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -9245,11 +9244,11 @@
       <c r="U47" s="26"/>
       <c r="V47" s="27"/>
       <c r="W47" s="27"/>
-      <c r="X47" s="176" t="s">
+      <c r="X47" s="185" t="s">
         <v>81</v>
       </c>
-      <c r="Y47" s="176"/>
-      <c r="Z47" s="176"/>
+      <c r="Y47" s="185"/>
+      <c r="Z47" s="185"/>
       <c r="AA47" s="27"/>
       <c r="AB47" s="27"/>
       <c r="AC47" s="85"/>
@@ -9282,25 +9281,25 @@
       <c r="BD47" s="4"/>
       <c r="BE47" s="4"/>
     </row>
-    <row r="48" spans="1:57" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="177" t="s">
+    <row r="48" spans="1:57" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="186" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="177"/>
-      <c r="C48" s="177"/>
-      <c r="D48" s="177"/>
-      <c r="E48" s="177"/>
-      <c r="F48" s="177"/>
-      <c r="G48" s="177"/>
-      <c r="H48" s="177"/>
-      <c r="I48" s="177"/>
-      <c r="J48" s="177"/>
-      <c r="K48" s="177"/>
-      <c r="L48" s="177"/>
-      <c r="M48" s="177"/>
-      <c r="N48" s="177"/>
-      <c r="O48" s="177"/>
-      <c r="P48" s="177"/>
+      <c r="B48" s="186"/>
+      <c r="C48" s="186"/>
+      <c r="D48" s="186"/>
+      <c r="E48" s="186"/>
+      <c r="F48" s="186"/>
+      <c r="G48" s="186"/>
+      <c r="H48" s="186"/>
+      <c r="I48" s="186"/>
+      <c r="J48" s="186"/>
+      <c r="K48" s="186"/>
+      <c r="L48" s="186"/>
+      <c r="M48" s="186"/>
+      <c r="N48" s="186"/>
+      <c r="O48" s="186"/>
+      <c r="P48" s="186"/>
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
@@ -9347,7 +9346,7 @@
       <c r="BD48" s="4"/>
       <c r="BE48" s="4"/>
     </row>
-    <row r="49" spans="1:58" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:58" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="55" t="s">
         <v>84</v>
       </c>
@@ -9444,7 +9443,7 @@
       <c r="BD49" s="4"/>
       <c r="BE49" s="4"/>
     </row>
-    <row r="50" spans="1:58" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:58" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="89">
         <v>1</v>
       </c>
@@ -9545,7 +9544,7 @@
       <c r="BD50" s="4"/>
       <c r="BE50" s="4"/>
     </row>
-    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A51" s="89">
         <v>2</v>
       </c>
@@ -9642,7 +9641,7 @@
       <c r="BD51" s="4"/>
       <c r="BE51" s="4"/>
     </row>
-    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A52" s="89">
         <v>3</v>
       </c>
@@ -9702,13 +9701,13 @@
       <c r="S52" s="4"/>
       <c r="T52" s="4"/>
       <c r="U52" s="26"/>
-      <c r="V52" s="178" t="s">
+      <c r="V52" s="187" t="s">
         <v>5</v>
       </c>
-      <c r="W52" s="178"/>
-      <c r="X52" s="178"/>
-      <c r="Y52" s="178"/>
-      <c r="Z52" s="178"/>
+      <c r="W52" s="187"/>
+      <c r="X52" s="187"/>
+      <c r="Y52" s="187"/>
+      <c r="Z52" s="187"/>
       <c r="AA52" s="27"/>
       <c r="AB52" s="27"/>
       <c r="AC52" s="85"/>
@@ -9741,7 +9740,7 @@
       <c r="BD52" s="4"/>
       <c r="BE52" s="4"/>
     </row>
-    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A53" s="89">
         <v>4</v>
       </c>
@@ -9840,7 +9839,7 @@
       <c r="BD53" s="4"/>
       <c r="BE53" s="4"/>
     </row>
-    <row r="54" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A54" s="89">
         <v>5</v>
       </c>
@@ -9945,7 +9944,7 @@
       <c r="BD54" s="4"/>
       <c r="BE54" s="4"/>
     </row>
-    <row r="55" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A55" s="106">
         <v>6</v>
       </c>
@@ -10042,7 +10041,7 @@
       <c r="BD55" s="4"/>
       <c r="BE55" s="4"/>
     </row>
-    <row r="56" spans="1:58" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:58" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="109" t="s">
         <v>104</v>
       </c>
@@ -10147,7 +10146,7 @@
       <c r="BE56" s="4"/>
       <c r="BF56" s="4"/>
     </row>
-    <row r="57" spans="1:58" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:58" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>105</v>
       </c>
@@ -10222,7 +10221,7 @@
       <c r="BE57" s="4"/>
       <c r="BF57" s="4"/>
     </row>
-    <row r="58" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -10295,24 +10294,24 @@
       <c r="BE58" s="4"/>
       <c r="BF58" s="4"/>
     </row>
-    <row r="59" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A59" s="179" t="s">
+    <row r="59" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A59" s="188" t="s">
         <v>107</v>
       </c>
-      <c r="B59" s="179"/>
-      <c r="C59" s="179"/>
-      <c r="D59" s="179"/>
-      <c r="E59" s="179"/>
-      <c r="F59" s="179"/>
-      <c r="G59" s="179"/>
-      <c r="H59" s="179"/>
-      <c r="I59" s="179"/>
-      <c r="J59" s="179"/>
-      <c r="K59" s="179"/>
-      <c r="L59" s="179"/>
-      <c r="M59" s="179"/>
-      <c r="N59" s="179"/>
-      <c r="O59" s="179"/>
+      <c r="B59" s="188"/>
+      <c r="C59" s="188"/>
+      <c r="D59" s="188"/>
+      <c r="E59" s="188"/>
+      <c r="F59" s="188"/>
+      <c r="G59" s="188"/>
+      <c r="H59" s="188"/>
+      <c r="I59" s="188"/>
+      <c r="J59" s="188"/>
+      <c r="K59" s="188"/>
+      <c r="L59" s="188"/>
+      <c r="M59" s="188"/>
+      <c r="N59" s="188"/>
+      <c r="O59" s="188"/>
       <c r="P59" s="4"/>
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
@@ -10370,7 +10369,7 @@
       <c r="BE59" s="4"/>
       <c r="BF59" s="4"/>
     </row>
-    <row r="60" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A60" s="55" t="s">
         <v>84</v>
       </c>
@@ -10473,7 +10472,7 @@
       <c r="BE60" s="4"/>
       <c r="BF60" s="4"/>
     </row>
-    <row r="61" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A61" s="89">
         <v>1</v>
       </c>
@@ -10569,7 +10568,7 @@
       <c r="BE61" s="4"/>
       <c r="BF61" s="4"/>
     </row>
-    <row r="62" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A62" s="89">
         <v>2</v>
       </c>
@@ -10665,7 +10664,7 @@
       <c r="BE62" s="4"/>
       <c r="BF62" s="4"/>
     </row>
-    <row r="63" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A63" s="89">
         <v>3</v>
       </c>
@@ -10761,7 +10760,7 @@
       <c r="BE63" s="4"/>
       <c r="BF63" s="4"/>
     </row>
-    <row r="64" spans="1:58" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:58" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="89">
         <v>4</v>
       </c>
@@ -10857,7 +10856,7 @@
       <c r="BE64" s="4"/>
       <c r="BF64" s="4"/>
     </row>
-    <row r="65" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" s="89">
         <v>5</v>
       </c>
@@ -10953,7 +10952,7 @@
       <c r="BE65" s="4"/>
       <c r="BF65" s="4"/>
     </row>
-    <row r="66" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" s="89">
         <v>6</v>
       </c>
@@ -11049,7 +11048,7 @@
       <c r="BE66" s="4"/>
       <c r="BF66" s="4"/>
     </row>
-    <row r="67" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" s="138" t="s">
         <v>118</v>
       </c>
@@ -11145,7 +11144,7 @@
       <c r="BE67" s="4"/>
       <c r="BF67" s="4"/>
     </row>
-    <row r="68" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" s="109" t="s">
         <v>119</v>
       </c>
@@ -11241,7 +11240,7 @@
       <c r="BE68" s="4"/>
       <c r="BF68" s="4"/>
     </row>
-    <row r="70" spans="1:58" s="162" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:58" s="162" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="143" t="s">
         <v>64</v>
       </c>
@@ -11389,7 +11388,7 @@
       </c>
       <c r="AX70" s="161"/>
     </row>
-    <row r="71" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="163">
         <f t="shared" ref="A71:A76" si="17">I33</f>
         <v>17.01308560441484</v>
@@ -11565,7 +11564,7 @@
       </c>
       <c r="AX71" s="164"/>
     </row>
-    <row r="72" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="163">
         <f t="shared" si="17"/>
         <v>18.736554961438362</v>
@@ -11665,7 +11664,7 @@
       <c r="AW72" s="149"/>
       <c r="AX72" s="164"/>
     </row>
-    <row r="73" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="163">
         <f t="shared" si="17"/>
         <v>21.415013228658076</v>
@@ -11765,7 +11764,7 @@
       <c r="AW73" s="149"/>
       <c r="AX73" s="164"/>
     </row>
-    <row r="74" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="163">
         <f t="shared" si="17"/>
         <v>23.899659713224764</v>
@@ -11865,7 +11864,7 @@
       <c r="AW74" s="149"/>
       <c r="AX74" s="164"/>
     </row>
-    <row r="75" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="163">
         <f t="shared" si="17"/>
         <v>26.603128665134808</v>
@@ -11965,7 +11964,7 @@
       <c r="AW75" s="149"/>
       <c r="AX75" s="164"/>
     </row>
-    <row r="76" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:58" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="163">
         <f t="shared" si="17"/>
         <v>29.139709765458161</v>
@@ -12067,21 +12066,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AD43:AL44"/>
+    <mergeCell ref="X47:Z47"/>
+    <mergeCell ref="A48:P48"/>
+    <mergeCell ref="V52:Z52"/>
+    <mergeCell ref="A59:O59"/>
+    <mergeCell ref="A31:R31"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="I40:M40"/>
+    <mergeCell ref="U43:AC44"/>
     <mergeCell ref="U5:AL7"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A31:R31"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="I40:M40"/>
-    <mergeCell ref="U43:AC44"/>
-    <mergeCell ref="AD43:AL44"/>
-    <mergeCell ref="X47:Z47"/>
-    <mergeCell ref="A48:P48"/>
-    <mergeCell ref="V52:Z52"/>
-    <mergeCell ref="A59:O59"/>
   </mergeCells>
   <conditionalFormatting sqref="X56">
     <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
@@ -12137,45 +12136,45 @@
   </sheetPr>
   <dimension ref="A1:BE76"/>
   <sheetViews>
-    <sheetView topLeftCell="B57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="16.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="2" customWidth="1"/>
+    <col min="7" max="8" width="16.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="2" customWidth="1"/>
     <col min="15" max="15" width="11" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" style="2" customWidth="1"/>
     <col min="17" max="17" width="11" style="2" customWidth="1"/>
-    <col min="18" max="21" width="11.6640625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="22.33203125" style="2" customWidth="1"/>
-    <col min="23" max="25" width="11.6640625" style="2" customWidth="1"/>
-    <col min="26" max="26" width="21.33203125" style="2" customWidth="1"/>
-    <col min="27" max="34" width="11.6640625" style="2" customWidth="1"/>
-    <col min="35" max="35" width="13.33203125" style="2" customWidth="1"/>
-    <col min="36" max="36" width="14.6640625" style="2" customWidth="1"/>
-    <col min="37" max="37" width="11.6640625" style="2" customWidth="1"/>
-    <col min="38" max="38" width="9.44140625" style="2" customWidth="1"/>
-    <col min="39" max="39" width="8.33203125" style="2" customWidth="1"/>
-    <col min="40" max="40" width="7.44140625" style="2" customWidth="1"/>
-    <col min="41" max="42" width="8.6640625" style="2"/>
-    <col min="43" max="43" width="8.44140625" style="2" customWidth="1"/>
-    <col min="44" max="16384" width="8.6640625" style="2"/>
+    <col min="18" max="21" width="11.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="22.28515625" style="2" customWidth="1"/>
+    <col min="23" max="25" width="11.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="21.28515625" style="2" customWidth="1"/>
+    <col min="27" max="34" width="11.7109375" style="2" customWidth="1"/>
+    <col min="35" max="35" width="13.28515625" style="2" customWidth="1"/>
+    <col min="36" max="36" width="14.7109375" style="2" customWidth="1"/>
+    <col min="37" max="37" width="11.7109375" style="2" customWidth="1"/>
+    <col min="38" max="38" width="9.42578125" style="2" customWidth="1"/>
+    <col min="39" max="39" width="8.28515625" style="2" customWidth="1"/>
+    <col min="40" max="40" width="7.42578125" style="2" customWidth="1"/>
+    <col min="41" max="42" width="8.7109375" style="2"/>
+    <col min="43" max="43" width="8.42578125" style="2" customWidth="1"/>
+    <col min="44" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -12236,7 +12235,7 @@
       <c r="BD1" s="4"/>
       <c r="BE1" s="4"/>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
         <v>1</v>
@@ -12297,7 +12296,7 @@
       <c r="BD2" s="4"/>
       <c r="BE2" s="4"/>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>2</v>
@@ -12358,7 +12357,7 @@
       <c r="BD3" s="4"/>
       <c r="BE3" s="4"/>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -12417,7 +12416,7 @@
       <c r="BD4" s="4"/>
       <c r="BE4" s="4"/>
     </row>
-    <row r="5" spans="1:57" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:57" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -12438,25 +12437,25 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
-      <c r="U5" s="185" t="s">
+      <c r="U5" s="175" t="s">
         <v>148</v>
       </c>
-      <c r="V5" s="185"/>
-      <c r="W5" s="185"/>
-      <c r="X5" s="185"/>
-      <c r="Y5" s="185"/>
-      <c r="Z5" s="185"/>
-      <c r="AA5" s="185"/>
-      <c r="AB5" s="185"/>
-      <c r="AC5" s="185"/>
-      <c r="AD5" s="185"/>
-      <c r="AE5" s="185"/>
-      <c r="AF5" s="185"/>
-      <c r="AG5" s="185"/>
-      <c r="AH5" s="185"/>
-      <c r="AI5" s="185"/>
-      <c r="AJ5" s="185"/>
-      <c r="AK5" s="185"/>
+      <c r="V5" s="175"/>
+      <c r="W5" s="175"/>
+      <c r="X5" s="175"/>
+      <c r="Y5" s="175"/>
+      <c r="Z5" s="175"/>
+      <c r="AA5" s="175"/>
+      <c r="AB5" s="175"/>
+      <c r="AC5" s="175"/>
+      <c r="AD5" s="175"/>
+      <c r="AE5" s="175"/>
+      <c r="AF5" s="175"/>
+      <c r="AG5" s="175"/>
+      <c r="AH5" s="175"/>
+      <c r="AI5" s="175"/>
+      <c r="AJ5" s="175"/>
+      <c r="AK5" s="175"/>
       <c r="AL5" s="4"/>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
@@ -12478,7 +12477,7 @@
       <c r="BD5" s="4"/>
       <c r="BE5" s="4"/>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -12499,23 +12498,23 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
-      <c r="U6" s="185"/>
-      <c r="V6" s="185"/>
-      <c r="W6" s="185"/>
-      <c r="X6" s="185"/>
-      <c r="Y6" s="185"/>
-      <c r="Z6" s="185"/>
-      <c r="AA6" s="185"/>
-      <c r="AB6" s="185"/>
-      <c r="AC6" s="185"/>
-      <c r="AD6" s="185"/>
-      <c r="AE6" s="185"/>
-      <c r="AF6" s="185"/>
-      <c r="AG6" s="185"/>
-      <c r="AH6" s="185"/>
-      <c r="AI6" s="185"/>
-      <c r="AJ6" s="185"/>
-      <c r="AK6" s="185"/>
+      <c r="U6" s="175"/>
+      <c r="V6" s="175"/>
+      <c r="W6" s="175"/>
+      <c r="X6" s="175"/>
+      <c r="Y6" s="175"/>
+      <c r="Z6" s="175"/>
+      <c r="AA6" s="175"/>
+      <c r="AB6" s="175"/>
+      <c r="AC6" s="175"/>
+      <c r="AD6" s="175"/>
+      <c r="AE6" s="175"/>
+      <c r="AF6" s="175"/>
+      <c r="AG6" s="175"/>
+      <c r="AH6" s="175"/>
+      <c r="AI6" s="175"/>
+      <c r="AJ6" s="175"/>
+      <c r="AK6" s="175"/>
       <c r="AL6" s="4"/>
       <c r="AM6" s="4"/>
       <c r="AN6" s="4"/>
@@ -12537,11 +12536,11 @@
       <c r="BD6" s="4"/>
       <c r="BE6" s="4"/>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A7" s="186"/>
-      <c r="B7" s="186"/>
-      <c r="C7" s="186"/>
-      <c r="D7" s="186"/>
+    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A7" s="176"/>
+      <c r="B7" s="176"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
       <c r="E7" s="4"/>
       <c r="F7" s="8" t="s">
         <v>5</v>
@@ -12560,23 +12559,23 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
-      <c r="U7" s="185"/>
-      <c r="V7" s="185"/>
-      <c r="W7" s="185"/>
-      <c r="X7" s="185"/>
-      <c r="Y7" s="185"/>
-      <c r="Z7" s="185"/>
-      <c r="AA7" s="185"/>
-      <c r="AB7" s="185"/>
-      <c r="AC7" s="185"/>
-      <c r="AD7" s="185"/>
-      <c r="AE7" s="185"/>
-      <c r="AF7" s="185"/>
-      <c r="AG7" s="185"/>
-      <c r="AH7" s="185"/>
-      <c r="AI7" s="185"/>
-      <c r="AJ7" s="185"/>
-      <c r="AK7" s="185"/>
+      <c r="U7" s="175"/>
+      <c r="V7" s="175"/>
+      <c r="W7" s="175"/>
+      <c r="X7" s="175"/>
+      <c r="Y7" s="175"/>
+      <c r="Z7" s="175"/>
+      <c r="AA7" s="175"/>
+      <c r="AB7" s="175"/>
+      <c r="AC7" s="175"/>
+      <c r="AD7" s="175"/>
+      <c r="AE7" s="175"/>
+      <c r="AF7" s="175"/>
+      <c r="AG7" s="175"/>
+      <c r="AH7" s="175"/>
+      <c r="AI7" s="175"/>
+      <c r="AJ7" s="175"/>
+      <c r="AK7" s="175"/>
       <c r="AL7" s="4"/>
       <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
@@ -12598,7 +12597,7 @@
       <c r="BD7" s="4"/>
       <c r="BE7" s="4"/>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
@@ -12668,7 +12667,7 @@
       <c r="BD8" s="4"/>
       <c r="BE8" s="4"/>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>10</v>
       </c>
@@ -12744,7 +12743,7 @@
       <c r="BD9" s="4"/>
       <c r="BE9" s="4"/>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>16</v>
       </c>
@@ -12819,7 +12818,7 @@
       <c r="BD10" s="4"/>
       <c r="BE10" s="4"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>20</v>
       </c>
@@ -12900,7 +12899,7 @@
       <c r="BD11" s="4"/>
       <c r="BE11" s="4"/>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -12981,7 +12980,7 @@
       <c r="BD12" s="4"/>
       <c r="BE12" s="4"/>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>28</v>
       </c>
@@ -13062,7 +13061,7 @@
       <c r="BD13" s="4"/>
       <c r="BE13" s="4"/>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:57" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>31</v>
       </c>
@@ -13143,7 +13142,7 @@
       <c r="BD14" s="4"/>
       <c r="BE14" s="4"/>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:57" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
         <v>35</v>
       </c>
@@ -13211,7 +13210,7 @@
       <c r="BD15" s="4"/>
       <c r="BE15" s="4"/>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A16" s="43"/>
       <c r="B16" s="43"/>
       <c r="C16" s="4"/>
@@ -13270,12 +13269,12 @@
       <c r="BD16" s="4"/>
       <c r="BE16" s="4"/>
     </row>
-    <row r="17" spans="1:57" ht="15.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A17" s="187" t="s">
+    <row r="17" spans="1:57" ht="15.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A17" s="177" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="187"/>
-      <c r="C17" s="187"/>
+      <c r="B17" s="177"/>
+      <c r="C17" s="177"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -13331,7 +13330,7 @@
       <c r="BD17" s="4"/>
       <c r="BE17" s="4"/>
     </row>
-    <row r="18" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="12"/>
       <c r="C18" s="45"/>
@@ -13390,12 +13389,11 @@
       <c r="BD18" s="4"/>
       <c r="BE18" s="4"/>
     </row>
-    <row r="19" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="47">
-        <f>1/453.59237</f>
         <v>2.2046226218487759E-3</v>
       </c>
       <c r="C19" s="48" t="s">
@@ -13456,7 +13454,7 @@
       <c r="BD19" s="4"/>
       <c r="BE19" s="4"/>
     </row>
-    <row r="20" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
         <v>38</v>
       </c>
@@ -13521,7 +13519,7 @@
       <c r="BD20" s="4"/>
       <c r="BE20" s="4"/>
     </row>
-    <row r="21" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
         <v>41</v>
       </c>
@@ -13586,7 +13584,7 @@
       <c r="BD21" s="4"/>
       <c r="BE21" s="4"/>
     </row>
-    <row r="22" spans="1:57" ht="17.399999999999999" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:57" ht="18" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
         <v>43</v>
       </c>
@@ -13652,12 +13650,12 @@
       <c r="BD22" s="4"/>
       <c r="BE22" s="4"/>
     </row>
-    <row r="23" spans="1:57" ht="17.399999999999999" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A23" s="188" t="s">
+    <row r="23" spans="1:57" ht="18" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A23" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="188"/>
-      <c r="C23" s="188"/>
+      <c r="B23" s="178"/>
+      <c r="C23" s="178"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -13713,7 +13711,7 @@
       <c r="BD23" s="4"/>
       <c r="BE23" s="4"/>
     </row>
-    <row r="24" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
         <v>46</v>
       </c>
@@ -13779,7 +13777,7 @@
       <c r="BD24" s="4"/>
       <c r="BE24" s="4"/>
     </row>
-    <row r="25" spans="1:57" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:57" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
         <v>48</v>
       </c>
@@ -13844,12 +13842,12 @@
       <c r="BD25" s="4"/>
       <c r="BE25" s="4"/>
     </row>
-    <row r="26" spans="1:57" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A26" s="188" t="s">
+    <row r="26" spans="1:57" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A26" s="178" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="188"/>
-      <c r="C26" s="188"/>
+      <c r="B26" s="178"/>
+      <c r="C26" s="178"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -13905,7 +13903,7 @@
       <c r="BD26" s="4"/>
       <c r="BE26" s="4"/>
     </row>
-    <row r="27" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
         <v>51</v>
       </c>
@@ -13967,7 +13965,7 @@
       <c r="BC27" s="4"/>
       <c r="BD27" s="4"/>
     </row>
-    <row r="28" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:57" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="51" t="s">
         <v>52</v>
       </c>
@@ -14031,7 +14029,7 @@
       <c r="BC28" s="4"/>
       <c r="BD28" s="4"/>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -14089,7 +14087,7 @@
       <c r="BC29" s="4"/>
       <c r="BD29" s="4"/>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -14147,27 +14145,27 @@
       <c r="BC30" s="4"/>
       <c r="BD30" s="4"/>
     </row>
-    <row r="31" spans="1:57" ht="18" x14ac:dyDescent="0.35">
-      <c r="A31" s="180" t="s">
+    <row r="31" spans="1:57" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="179" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="180"/>
-      <c r="C31" s="180"/>
-      <c r="D31" s="180"/>
-      <c r="E31" s="180"/>
-      <c r="F31" s="180"/>
-      <c r="G31" s="180"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="180"/>
-      <c r="J31" s="180"/>
-      <c r="K31" s="180"/>
-      <c r="L31" s="180"/>
-      <c r="M31" s="180"/>
-      <c r="N31" s="180"/>
-      <c r="O31" s="180"/>
-      <c r="P31" s="180"/>
-      <c r="Q31" s="180"/>
-      <c r="R31" s="180"/>
+      <c r="B31" s="179"/>
+      <c r="C31" s="179"/>
+      <c r="D31" s="179"/>
+      <c r="E31" s="179"/>
+      <c r="F31" s="179"/>
+      <c r="G31" s="179"/>
+      <c r="H31" s="179"/>
+      <c r="I31" s="179"/>
+      <c r="J31" s="179"/>
+      <c r="K31" s="179"/>
+      <c r="L31" s="179"/>
+      <c r="M31" s="179"/>
+      <c r="N31" s="179"/>
+      <c r="O31" s="179"/>
+      <c r="P31" s="179"/>
+      <c r="Q31" s="179"/>
+      <c r="R31" s="179"/>
       <c r="S31" s="54"/>
       <c r="T31" s="54"/>
       <c r="U31" s="26"/>
@@ -14207,7 +14205,7 @@
       <c r="BC31" s="4"/>
       <c r="BD31" s="4"/>
     </row>
-    <row r="32" spans="1:57" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:57" ht="63" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
         <v>56</v>
       </c>
@@ -14301,7 +14299,7 @@
       <c r="BC32" s="4"/>
       <c r="BD32" s="4"/>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A33" s="59">
         <v>1</v>
       </c>
@@ -14402,7 +14400,7 @@
       <c r="BC33" s="4"/>
       <c r="BD33" s="4"/>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A34" s="59">
         <v>2</v>
       </c>
@@ -14503,7 +14501,7 @@
       <c r="BC34" s="4"/>
       <c r="BD34" s="4"/>
     </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A35" s="59">
         <v>3</v>
       </c>
@@ -14604,7 +14602,7 @@
       <c r="BC35" s="4"/>
       <c r="BD35" s="4"/>
     </row>
-    <row r="36" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A36" s="59">
         <v>4</v>
       </c>
@@ -14705,7 +14703,7 @@
       <c r="BC36" s="4"/>
       <c r="BD36" s="4"/>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A37" s="59">
         <v>5</v>
       </c>
@@ -14806,7 +14804,7 @@
       <c r="BC37" s="4"/>
       <c r="BD37" s="4"/>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A38" s="70"/>
       <c r="B38" s="71">
         <v>35</v>
@@ -14905,22 +14903,22 @@
       <c r="BC38" s="4"/>
       <c r="BD38" s="4"/>
     </row>
-    <row r="39" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="181" t="s">
+    <row r="39" spans="1:56" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="180" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="181"/>
-      <c r="C39" s="181"/>
-      <c r="D39" s="181"/>
-      <c r="E39" s="181"/>
-      <c r="F39" s="181"/>
-      <c r="G39" s="181"/>
-      <c r="H39" s="181"/>
-      <c r="I39" s="181"/>
-      <c r="J39" s="181"/>
-      <c r="K39" s="181"/>
-      <c r="L39" s="181"/>
-      <c r="M39" s="181"/>
+      <c r="B39" s="180"/>
+      <c r="C39" s="180"/>
+      <c r="D39" s="180"/>
+      <c r="E39" s="180"/>
+      <c r="F39" s="180"/>
+      <c r="G39" s="180"/>
+      <c r="H39" s="180"/>
+      <c r="I39" s="180"/>
+      <c r="J39" s="180"/>
+      <c r="K39" s="180"/>
+      <c r="L39" s="180"/>
+      <c r="M39" s="180"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
@@ -14967,7 +14965,7 @@
       <c r="BC39" s="4"/>
       <c r="BD39" s="4"/>
     </row>
-    <row r="40" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="56" t="s">
         <v>56</v>
       </c>
@@ -14977,20 +14975,20 @@
       <c r="C40" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="182" t="s">
+      <c r="D40" s="181" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="182"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="182"/>
-      <c r="H40" s="182"/>
-      <c r="I40" s="183" t="s">
+      <c r="E40" s="181"/>
+      <c r="F40" s="181"/>
+      <c r="G40" s="181"/>
+      <c r="H40" s="181"/>
+      <c r="I40" s="182" t="s">
         <v>78</v>
       </c>
-      <c r="J40" s="183"/>
-      <c r="K40" s="183"/>
-      <c r="L40" s="183"/>
-      <c r="M40" s="183"/>
+      <c r="J40" s="182"/>
+      <c r="K40" s="182"/>
+      <c r="L40" s="182"/>
+      <c r="M40" s="182"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
@@ -15035,7 +15033,7 @@
       <c r="BC40" s="4"/>
       <c r="BD40" s="4"/>
     </row>
-    <row r="41" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A41" s="74">
         <v>1</v>
       </c>
@@ -15113,7 +15111,7 @@
       <c r="BC41" s="4"/>
       <c r="BD41" s="4"/>
     </row>
-    <row r="42" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A42" s="74">
         <v>2</v>
       </c>
@@ -15193,7 +15191,7 @@
       <c r="BC42" s="4"/>
       <c r="BD42" s="4"/>
     </row>
-    <row r="43" spans="1:56" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:56" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="74">
         <v>3</v>
       </c>
@@ -15236,27 +15234,27 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
-      <c r="U43" s="184" t="s">
+      <c r="U43" s="183" t="s">
         <v>79</v>
       </c>
-      <c r="V43" s="184"/>
-      <c r="W43" s="184"/>
-      <c r="X43" s="184"/>
-      <c r="Y43" s="184"/>
-      <c r="Z43" s="184"/>
-      <c r="AA43" s="184"/>
-      <c r="AB43" s="184"/>
-      <c r="AC43" s="175" t="s">
+      <c r="V43" s="183"/>
+      <c r="W43" s="183"/>
+      <c r="X43" s="183"/>
+      <c r="Y43" s="183"/>
+      <c r="Z43" s="183"/>
+      <c r="AA43" s="183"/>
+      <c r="AB43" s="183"/>
+      <c r="AC43" s="184" t="s">
         <v>80</v>
       </c>
-      <c r="AD43" s="175"/>
-      <c r="AE43" s="175"/>
-      <c r="AF43" s="175"/>
-      <c r="AG43" s="175"/>
-      <c r="AH43" s="175"/>
-      <c r="AI43" s="175"/>
-      <c r="AJ43" s="175"/>
-      <c r="AK43" s="175"/>
+      <c r="AD43" s="184"/>
+      <c r="AE43" s="184"/>
+      <c r="AF43" s="184"/>
+      <c r="AG43" s="184"/>
+      <c r="AH43" s="184"/>
+      <c r="AI43" s="184"/>
+      <c r="AJ43" s="184"/>
+      <c r="AK43" s="184"/>
       <c r="AL43" s="4"/>
       <c r="AM43" s="4"/>
       <c r="AN43" s="4"/>
@@ -15277,7 +15275,7 @@
       <c r="BC43" s="4"/>
       <c r="BD43" s="4"/>
     </row>
-    <row r="44" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="74">
         <v>4</v>
       </c>
@@ -15320,23 +15318,23 @@
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
-      <c r="U44" s="184"/>
-      <c r="V44" s="184"/>
-      <c r="W44" s="184"/>
-      <c r="X44" s="184"/>
-      <c r="Y44" s="184"/>
-      <c r="Z44" s="184"/>
-      <c r="AA44" s="184"/>
-      <c r="AB44" s="184"/>
-      <c r="AC44" s="175"/>
-      <c r="AD44" s="175"/>
-      <c r="AE44" s="175"/>
-      <c r="AF44" s="175"/>
-      <c r="AG44" s="175"/>
-      <c r="AH44" s="175"/>
-      <c r="AI44" s="175"/>
-      <c r="AJ44" s="175"/>
-      <c r="AK44" s="175"/>
+      <c r="U44" s="183"/>
+      <c r="V44" s="183"/>
+      <c r="W44" s="183"/>
+      <c r="X44" s="183"/>
+      <c r="Y44" s="183"/>
+      <c r="Z44" s="183"/>
+      <c r="AA44" s="183"/>
+      <c r="AB44" s="183"/>
+      <c r="AC44" s="184"/>
+      <c r="AD44" s="184"/>
+      <c r="AE44" s="184"/>
+      <c r="AF44" s="184"/>
+      <c r="AG44" s="184"/>
+      <c r="AH44" s="184"/>
+      <c r="AI44" s="184"/>
+      <c r="AJ44" s="184"/>
+      <c r="AK44" s="184"/>
       <c r="AL44" s="4"/>
       <c r="AM44" s="4"/>
       <c r="AN44" s="4"/>
@@ -15357,7 +15355,7 @@
       <c r="BC44" s="4"/>
       <c r="BD44" s="4"/>
     </row>
-    <row r="45" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="74">
         <v>5</v>
       </c>
@@ -15437,7 +15435,7 @@
       <c r="BC45" s="4"/>
       <c r="BD45" s="4"/>
     </row>
-    <row r="46" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="74">
         <v>5</v>
       </c>
@@ -15517,7 +15515,7 @@
       <c r="BC46" s="4"/>
       <c r="BD46" s="4"/>
     </row>
-    <row r="47" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -15541,11 +15539,11 @@
       <c r="U47" s="26"/>
       <c r="V47" s="27"/>
       <c r="W47" s="27"/>
-      <c r="X47" s="176" t="s">
+      <c r="X47" s="185" t="s">
         <v>81</v>
       </c>
-      <c r="Y47" s="176"/>
-      <c r="Z47" s="176"/>
+      <c r="Y47" s="185"/>
+      <c r="Z47" s="185"/>
       <c r="AA47" s="27"/>
       <c r="AB47" s="85"/>
       <c r="AC47" s="27"/>
@@ -15577,25 +15575,25 @@
       <c r="BC47" s="4"/>
       <c r="BD47" s="4"/>
     </row>
-    <row r="48" spans="1:56" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="177" t="s">
+    <row r="48" spans="1:56" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="186" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="177"/>
-      <c r="C48" s="177"/>
-      <c r="D48" s="177"/>
-      <c r="E48" s="177"/>
-      <c r="F48" s="177"/>
-      <c r="G48" s="177"/>
-      <c r="H48" s="177"/>
-      <c r="I48" s="177"/>
-      <c r="J48" s="177"/>
-      <c r="K48" s="177"/>
-      <c r="L48" s="177"/>
-      <c r="M48" s="177"/>
-      <c r="N48" s="177"/>
-      <c r="O48" s="177"/>
-      <c r="P48" s="177"/>
+      <c r="B48" s="186"/>
+      <c r="C48" s="186"/>
+      <c r="D48" s="186"/>
+      <c r="E48" s="186"/>
+      <c r="F48" s="186"/>
+      <c r="G48" s="186"/>
+      <c r="H48" s="186"/>
+      <c r="I48" s="186"/>
+      <c r="J48" s="186"/>
+      <c r="K48" s="186"/>
+      <c r="L48" s="186"/>
+      <c r="M48" s="186"/>
+      <c r="N48" s="186"/>
+      <c r="O48" s="186"/>
+      <c r="P48" s="186"/>
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
@@ -15641,7 +15639,7 @@
       <c r="BC48" s="4"/>
       <c r="BD48" s="4"/>
     </row>
-    <row r="49" spans="1:57" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:57" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="55" t="s">
         <v>84</v>
       </c>
@@ -15737,7 +15735,7 @@
       <c r="BC49" s="4"/>
       <c r="BD49" s="4"/>
     </row>
-    <row r="50" spans="1:57" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:57" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="89">
         <v>1</v>
       </c>
@@ -15837,7 +15835,7 @@
       <c r="BC50" s="4"/>
       <c r="BD50" s="4"/>
     </row>
-    <row r="51" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A51" s="89">
         <v>2</v>
       </c>
@@ -15933,7 +15931,7 @@
       <c r="BC51" s="4"/>
       <c r="BD51" s="4"/>
     </row>
-    <row r="52" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A52" s="89">
         <v>3</v>
       </c>
@@ -15993,13 +15991,13 @@
       <c r="S52" s="4"/>
       <c r="T52" s="4"/>
       <c r="U52" s="26"/>
-      <c r="V52" s="178" t="s">
+      <c r="V52" s="187" t="s">
         <v>5</v>
       </c>
-      <c r="W52" s="178"/>
-      <c r="X52" s="178"/>
-      <c r="Y52" s="178"/>
-      <c r="Z52" s="178"/>
+      <c r="W52" s="187"/>
+      <c r="X52" s="187"/>
+      <c r="Y52" s="187"/>
+      <c r="Z52" s="187"/>
       <c r="AA52" s="27"/>
       <c r="AB52" s="85"/>
       <c r="AC52" s="27"/>
@@ -16031,7 +16029,7 @@
       <c r="BC52" s="4"/>
       <c r="BD52" s="4"/>
     </row>
-    <row r="53" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A53" s="89">
         <v>4</v>
       </c>
@@ -16129,7 +16127,7 @@
       <c r="BC53" s="4"/>
       <c r="BD53" s="4"/>
     </row>
-    <row r="54" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A54" s="89">
         <v>5</v>
       </c>
@@ -16233,7 +16231,7 @@
       <c r="BC54" s="4"/>
       <c r="BD54" s="4"/>
     </row>
-    <row r="55" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A55" s="106">
         <v>6</v>
       </c>
@@ -16329,7 +16327,7 @@
       <c r="BC55" s="4"/>
       <c r="BD55" s="4"/>
     </row>
-    <row r="56" spans="1:57" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:57" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="109" t="s">
         <v>104</v>
       </c>
@@ -16433,7 +16431,7 @@
       <c r="BD56" s="4"/>
       <c r="BE56" s="4"/>
     </row>
-    <row r="57" spans="1:57" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:57" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>105</v>
       </c>
@@ -16507,7 +16505,7 @@
       <c r="BD57" s="4"/>
       <c r="BE57" s="4"/>
     </row>
-    <row r="58" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -16579,24 +16577,24 @@
       <c r="BD58" s="4"/>
       <c r="BE58" s="4"/>
     </row>
-    <row r="59" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A59" s="179" t="s">
+    <row r="59" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A59" s="188" t="s">
         <v>107</v>
       </c>
-      <c r="B59" s="179"/>
-      <c r="C59" s="179"/>
-      <c r="D59" s="179"/>
-      <c r="E59" s="179"/>
-      <c r="F59" s="179"/>
-      <c r="G59" s="179"/>
-      <c r="H59" s="179"/>
-      <c r="I59" s="179"/>
-      <c r="J59" s="179"/>
-      <c r="K59" s="179"/>
-      <c r="L59" s="179"/>
-      <c r="M59" s="179"/>
-      <c r="N59" s="179"/>
-      <c r="O59" s="179"/>
+      <c r="B59" s="188"/>
+      <c r="C59" s="188"/>
+      <c r="D59" s="188"/>
+      <c r="E59" s="188"/>
+      <c r="F59" s="188"/>
+      <c r="G59" s="188"/>
+      <c r="H59" s="188"/>
+      <c r="I59" s="188"/>
+      <c r="J59" s="188"/>
+      <c r="K59" s="188"/>
+      <c r="L59" s="188"/>
+      <c r="M59" s="188"/>
+      <c r="N59" s="188"/>
+      <c r="O59" s="188"/>
       <c r="P59" s="4"/>
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
@@ -16653,7 +16651,7 @@
       <c r="BD59" s="4"/>
       <c r="BE59" s="4"/>
     </row>
-    <row r="60" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A60" s="55" t="s">
         <v>84</v>
       </c>
@@ -16755,7 +16753,7 @@
       <c r="BD60" s="4"/>
       <c r="BE60" s="4"/>
     </row>
-    <row r="61" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A61" s="89">
         <v>1</v>
       </c>
@@ -16850,7 +16848,7 @@
       <c r="BD61" s="4"/>
       <c r="BE61" s="4"/>
     </row>
-    <row r="62" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A62" s="89">
         <v>2</v>
       </c>
@@ -16945,7 +16943,7 @@
       <c r="BD62" s="4"/>
       <c r="BE62" s="4"/>
     </row>
-    <row r="63" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A63" s="89">
         <v>3</v>
       </c>
@@ -17040,7 +17038,7 @@
       <c r="BD63" s="4"/>
       <c r="BE63" s="4"/>
     </row>
-    <row r="64" spans="1:57" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:57" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="89">
         <v>4</v>
       </c>
@@ -17135,7 +17133,7 @@
       <c r="BD64" s="4"/>
       <c r="BE64" s="4"/>
     </row>
-    <row r="65" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A65" s="89">
         <v>5</v>
       </c>
@@ -17230,7 +17228,7 @@
       <c r="BD65" s="4"/>
       <c r="BE65" s="4"/>
     </row>
-    <row r="66" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A66" s="89">
         <v>6</v>
       </c>
@@ -17325,7 +17323,7 @@
       <c r="BD66" s="4"/>
       <c r="BE66" s="4"/>
     </row>
-    <row r="67" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A67" s="138" t="s">
         <v>118</v>
       </c>
@@ -17420,7 +17418,7 @@
       <c r="BD67" s="4"/>
       <c r="BE67" s="4"/>
     </row>
-    <row r="68" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A68" s="109" t="s">
         <v>119</v>
       </c>
@@ -17515,7 +17513,7 @@
       <c r="BD68" s="4"/>
       <c r="BE68" s="4"/>
     </row>
-    <row r="69" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>1</v>
       </c>
@@ -17643,7 +17641,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:57" s="162" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:57" s="162" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="143" t="s">
         <v>64</v>
       </c>
@@ -17790,7 +17788,7 @@
       </c>
       <c r="AW70" s="161"/>
     </row>
-    <row r="71" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="163">
         <f t="shared" ref="A71:A76" si="17">I33</f>
         <v>20.007722912874286</v>
@@ -17965,7 +17963,7 @@
       </c>
       <c r="AW71" s="164"/>
     </row>
-    <row r="72" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="163">
         <f t="shared" si="17"/>
         <v>23.620471108633257</v>
@@ -18064,7 +18062,7 @@
       <c r="AV72" s="149"/>
       <c r="AW72" s="164"/>
     </row>
-    <row r="73" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="163">
         <f t="shared" si="17"/>
         <v>27.258618248517067</v>
@@ -18163,7 +18161,7 @@
       <c r="AV73" s="149"/>
       <c r="AW73" s="164"/>
     </row>
-    <row r="74" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="163">
         <f t="shared" si="17"/>
         <v>29.38051419007007</v>
@@ -18262,7 +18260,7 @@
       <c r="AV74" s="149"/>
       <c r="AW74" s="164"/>
     </row>
-    <row r="75" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="163">
         <f t="shared" si="17"/>
         <v>32.741633515543377</v>
@@ -18361,7 +18359,7 @@
       <c r="AV75" s="149"/>
       <c r="AW75" s="164"/>
     </row>
-    <row r="76" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:57" s="172" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="163">
         <f t="shared" si="17"/>
         <v>34.901150296083991</v>
@@ -18462,21 +18460,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AC43:AK44"/>
+    <mergeCell ref="X47:Z47"/>
+    <mergeCell ref="A48:P48"/>
+    <mergeCell ref="V52:Z52"/>
+    <mergeCell ref="A59:O59"/>
+    <mergeCell ref="A31:R31"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="I40:M40"/>
+    <mergeCell ref="U43:AB44"/>
     <mergeCell ref="U5:AK7"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A31:R31"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="I40:M40"/>
-    <mergeCell ref="U43:AB44"/>
-    <mergeCell ref="AC43:AK44"/>
-    <mergeCell ref="X47:Z47"/>
-    <mergeCell ref="A48:P48"/>
-    <mergeCell ref="V52:Z52"/>
-    <mergeCell ref="A59:O59"/>
   </mergeCells>
   <conditionalFormatting sqref="X56">
     <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThan">

</xml_diff>